<commit_message>
V:1.4 | Captura de error por conexion a base de datos y cierre de Inventor en caso de apertura del mismo
</commit_message>
<xml_diff>
--- a/despiece.xlsx
+++ b/despiece.xlsx
@@ -462,10 +462,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="C2" t="n">
-        <v>6125</v>
+        <v>5500</v>
       </c>
       <c r="D2" t="n">
         <v>100</v>
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C3" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="D3" t="n">
         <v>100</v>
@@ -494,10 +494,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="C4" t="n">
-        <v>6125</v>
+        <v>5500</v>
       </c>
       <c r="D4" t="n">
         <v>100</v>
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C5" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="D5" t="n">
         <v>100</v>
@@ -526,10 +526,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2800</v>
+        <v>1800</v>
       </c>
       <c r="C6" t="n">
-        <v>6125</v>
+        <v>5500</v>
       </c>
       <c r="D6" t="n">
         <v>100</v>
@@ -542,10 +542,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2800</v>
+        <v>1800</v>
       </c>
       <c r="C7" t="n">
-        <v>900</v>
+        <v>1400</v>
       </c>
       <c r="D7" t="n">
         <v>100</v>
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2800</v>
+        <v>1800</v>
       </c>
       <c r="C8" t="n">
-        <v>900</v>
+        <v>1400</v>
       </c>
       <c r="D8" t="n">
         <v>100</v>

</xml_diff>

<commit_message>
V:1.5 | Cambio en el estilo CSS de toda la aplicacion
</commit_message>
<xml_diff>
--- a/despiece.xlsx
+++ b/despiece.xlsx
@@ -462,10 +462,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1500</v>
+        <v>1250</v>
       </c>
       <c r="C2" t="n">
-        <v>5500</v>
+        <v>6000</v>
       </c>
       <c r="D2" t="n">
         <v>100</v>
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="C3" t="n">
-        <v>1500</v>
+        <v>1250</v>
       </c>
       <c r="D3" t="n">
         <v>100</v>
@@ -494,10 +494,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1500</v>
+        <v>1250</v>
       </c>
       <c r="C4" t="n">
-        <v>5500</v>
+        <v>6000</v>
       </c>
       <c r="D4" t="n">
         <v>100</v>
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="C5" t="n">
-        <v>1500</v>
+        <v>1250</v>
       </c>
       <c r="D5" t="n">
         <v>100</v>
@@ -526,10 +526,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1800</v>
+        <v>2300</v>
       </c>
       <c r="C6" t="n">
-        <v>5500</v>
+        <v>6000</v>
       </c>
       <c r="D6" t="n">
         <v>100</v>
@@ -542,10 +542,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1800</v>
+        <v>2300</v>
       </c>
       <c r="C7" t="n">
-        <v>1400</v>
+        <v>1150</v>
       </c>
       <c r="D7" t="n">
         <v>100</v>
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1800</v>
+        <v>2300</v>
       </c>
       <c r="C8" t="n">
-        <v>1400</v>
+        <v>1150</v>
       </c>
       <c r="D8" t="n">
         <v>100</v>

</xml_diff>